<commit_message>
Data import of standards, direct award and new framework and benchmark prices done.
Included additinoal values from RM3830 assessed value services and UoM.xlsx into the rates.csv file

fm_calculator fixed so it finds the right framework and benchmark values for a specific service

Priced at framework is now taken into account when checking if eligible for DA

Rubocop fixes and added the latest excel file

Fixed services.csv file

Added limits to string attributes in the migration
</commit_message>
<xml_diff>
--- a/data/facilities_management/RM3830 Direct Award Data (for Dev & Test).xlsx
+++ b/data/facilities_management/RM3830 Direct Award Data (for Dev & Test).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10715"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tariq/ccs/github/crown-marketplace/data/facilities_management/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/iceraluk/Projects/crown-marketplace/data/facilities_management/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0846C56-7B7E-3049-A712-067EE9686C26}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B8CB535-CAE1-9C42-877B-9C21B88EA553}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17040" activeTab="2" xr2:uid="{E52F7FF7-80D8-A545-86A4-0E8FF36F8E0B}"/>
+    <workbookView xWindow="6380" yWindow="460" windowWidth="28800" windowHeight="17040" xr2:uid="{E52F7FF7-80D8-A545-86A4-0E8FF36F8E0B}"/>
   </bookViews>
   <sheets>
     <sheet name="Prices" sheetId="1" r:id="rId1"/>
@@ -1062,9 +1062,9 @@
   </sheetPr>
   <dimension ref="A1:Q1145"/>
   <sheetViews>
-    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A238" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D258" sqref="D258"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.75" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
@@ -77848,8 +77848,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02F73148-05BF-EE45-AD1F-B3DF659C8157}">
   <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+    <sheetView topLeftCell="A5" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="11" x14ac:dyDescent="0.15"/>

</xml_diff>